<commit_message>
can retrive orders from api
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\prosjekter\kodeoppgave\Order-placement-system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EE096D-822C-44E7-93B5-E710D5D6E2D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFE1B61-59AC-4F8F-A6C2-E5D0D1608EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1068" yWindow="564" windowWidth="19008" windowHeight="9492" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Order" sheetId="1" r:id="rId1"/>
     <sheet name="Address" sheetId="5" r:id="rId2"/>
-    <sheet name="Order_Service" sheetId="4" r:id="rId3"/>
+    <sheet name="OrderJobService" sheetId="4" r:id="rId3"/>
     <sheet name="Customer" sheetId="2" r:id="rId4"/>
     <sheet name="JobService" sheetId="3" r:id="rId5"/>
   </sheets>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>id</t>
   </si>
@@ -70,23 +70,61 @@
     <t>order_id</t>
   </si>
   <si>
-    <t>service_id</t>
-  </si>
-  <si>
     <t>from_address_id</t>
   </si>
   <si>
     <t>to_address_id</t>
+  </si>
+  <si>
+    <t>job_service_id</t>
+  </si>
+  <si>
+    <t>street</t>
+  </si>
+  <si>
+    <t>zip_code</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>Veumveien 41G</t>
+  </si>
+  <si>
+    <t>Fredrikstad</t>
+  </si>
+  <si>
+    <t>Ekreveien 38A</t>
+  </si>
+  <si>
+    <t>Jørgen</t>
+  </si>
+  <si>
+    <t>Eriksen</t>
+  </si>
+  <si>
+    <t>jorgen.eriksen93@gmail.com</t>
+  </si>
+  <si>
+    <t>Kan være veiarbeid utenfor boligen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -109,13 +147,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperkobling" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -394,7 +436,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
@@ -406,7 +448,7 @@
     <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -417,10 +459,10 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>14</v>
-      </c>
-      <c r="D1" t="s">
-        <v>15</v>
       </c>
       <c r="E1" t="s">
         <v>9</v>
@@ -429,19 +471,88 @@
         <v>11</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>44479</v>
+      </c>
+      <c r="F2" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D042DC36-A08E-4160-B935-720922503CAC}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2">
+        <v>1613</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3">
+        <v>1613</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -451,7 +562,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -464,7 +575,7 @@
         <v>12</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -540,14 +651,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{479C4D33-D6DF-4BB9-9A9A-75D5997E46E5}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="5" max="5" width="24.88671875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -568,7 +680,27 @@
         <v>4</v>
       </c>
     </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>97498123</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{CD343ED4-319C-481F-B544-249839A16485}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>